<commit_message>
next gen stats added
</commit_message>
<xml_diff>
--- a/backend/data/odds/nfl odds 2022-23.xlsx
+++ b/backend/data/odds/nfl odds 2022-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8403595d4321e36a/Documents/Python/NFL/backend/data/odds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="410" documentId="11_0E25D3F6C7544E0F62355476585DCE3A87475678" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60DB672F-9951-4F30-85D7-E39DB1AE1A1B}"/>
+  <xr:revisionPtr revIDLastSave="412" documentId="11_0E25D3F6C7544E0F62355476585DCE3A87475678" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{438AE644-83BC-4882-9C41-8285FA5E9B10}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,7 +515,7 @@
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2608,10 +2608,10 @@
         <v>33</v>
       </c>
       <c r="C81">
-        <v>-315</v>
+        <v>-345</v>
       </c>
       <c r="D81">
-        <v>275</v>
+        <v>305</v>
       </c>
       <c r="E81">
         <v>7</v>

</xml_diff>